<commit_message>
added more university data
</commit_message>
<xml_diff>
--- a/LuminaUniversities.xlsx
+++ b/LuminaUniversities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAMZA\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40DD559C-E695-401B-88F8-9CB098411E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F922C6A7-A30C-434C-A8D1-3BD80062B2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB89910E-2519-499E-B587-9C93799E5226}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{FB89910E-2519-499E-B587-9C93799E5226}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>University</t>
   </si>
@@ -129,6 +129,27 @@
   </si>
   <si>
     <t>public</t>
+  </si>
+  <si>
+    <t>University of Health Sciences (UHS)</t>
+  </si>
+  <si>
+    <t>Bahauddin Zakariya Univeristy</t>
+  </si>
+  <si>
+    <t>Multan</t>
+  </si>
+  <si>
+    <t>UET</t>
+  </si>
+  <si>
+    <t>Sahiwal</t>
+  </si>
+  <si>
+    <t>University of Sahiwal</t>
+  </si>
+  <si>
+    <t>NUST</t>
   </si>
 </sst>
 </file>
@@ -500,15 +521,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0BDFA4-09A4-4C17-B2EF-01FFD73923FA}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
@@ -1054,6 +1075,65 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>50000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
@@ -1110,6 +1190,360 @@
         <v>1</v>
       </c>
       <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>40000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>54000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>54000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>120000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>30000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>200000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
         <v>1</v>
       </c>
     </row>
@@ -1127,15 +1561,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F87FBBC44E4C4647BA25B53146ABDD66" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d24a4fd5314d2cf9fe51300bc82172b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cc567431-2072-449e-9e63-2b585666d794" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbcd54e249b8179f2ac2fc8773779b15" ns3:_="">
     <xsd:import namespace="cc567431-2072-449e-9e63-2b585666d794"/>
@@ -1291,6 +1716,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E992717-7BA6-44D2-B372-85D6E9F9D4E4}">
   <ds:schemaRefs>
@@ -1308,14 +1742,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0849BD-654A-4E28-B32E-ADD8D49AA081}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AEE226B-2B0C-4204-9E72-265344CF3CCE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1331,4 +1757,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0849BD-654A-4E28-B32E-ADD8D49AA081}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>